<commit_message>
match 2016 12 04
</commit_message>
<xml_diff>
--- a/Education/Math_wrongs.xlsx
+++ b/Education/Math_wrongs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
   <si>
     <t>保留一位小数</t>
   </si>
@@ -378,7 +378,92 @@
     <t>0.92 ÷ 0.4 =</t>
   </si>
   <si>
-    <t>P34</t>
+    <t>0.125 × 5 =</t>
+  </si>
+  <si>
+    <t>1.5 ÷ 40 =</t>
+  </si>
+  <si>
+    <t>4.8 ÷ 60 =</t>
+  </si>
+  <si>
+    <t>8 ÷ 0.5 =</t>
+  </si>
+  <si>
+    <t>0.25 × 60 =</t>
+  </si>
+  <si>
+    <t>0.8 ÷ 0.01 =</t>
+  </si>
+  <si>
+    <t>3.2 ÷ 0.2 =</t>
+  </si>
+  <si>
+    <t>7.2 ÷ 0.4 =</t>
+  </si>
+  <si>
+    <t>3.7 ÷ 0.5 =</t>
+  </si>
+  <si>
+    <t>2.6 × 4 =</t>
+  </si>
+  <si>
+    <t>1.3 × 0.5 =</t>
+  </si>
+  <si>
+    <t>1.2 × 0.4 =</t>
+  </si>
+  <si>
+    <t>0.52b + 0.8b =</t>
+  </si>
+  <si>
+    <t>7.6 ÷ 0.2 =</t>
+  </si>
+  <si>
+    <t>0.75 ÷ 0.25 =</t>
+  </si>
+  <si>
+    <r>
+      <t>8.6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>χ -7χ = 32</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> χ =</t>
+  </si>
+  <si>
+    <t>9χ -4χ = 7.8</t>
+  </si>
+  <si>
+    <t>3.6 × 0.5 =</t>
+  </si>
+  <si>
+    <r>
+      <t>0.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>χ  = 16.4</t>
+    </r>
+  </si>
+  <si>
+    <t>3.4 ÷ 68 =</t>
+  </si>
+  <si>
+    <t>P49</t>
   </si>
 </sst>
 </file>
@@ -420,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -430,6 +515,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1119,6 +1207,95 @@
       <c r="C22" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>